<commit_message>
Updated readme, pdf cheat sheet
</commit_message>
<xml_diff>
--- a/documentation/Cheat_Sheet.xlsx
+++ b/documentation/Cheat_Sheet.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevSRClocal\UX\documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1403C0E1-DFE0-4EC1-8DD3-8F1CCFADD066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="3800" yWindow="3800" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Hoja1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -241,8 +247,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -253,14 +258,14 @@
     </font>
     <font>
       <sz val="18"/>
-      <color rgb="FF44546a"/>
+      <color rgb="FF44546A"/>
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
-      <color rgb="FF44546a"/>
+      <color rgb="FF44546A"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -293,7 +298,7 @@
       <right/>
       <top/>
       <bottom style="thick">
-        <color rgb="FF4472c4"/>
+        <color rgb="FF4472C4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -302,28 +307,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -334,10 +338,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -375,71 +379,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -467,7 +471,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -490,11 +494,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -503,13 +507,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -519,7 +523,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -528,7 +532,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -537,7 +541,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -545,10 +549,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -613,23 +617,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="4" width="24.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="31.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="20.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="31.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="24.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7265625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="27.75">
+    <row r="1" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -639,13 +644,13 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="25.5">
+    <row r="3" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -655,7 +660,7 @@
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -669,7 +674,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -683,7 +688,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
@@ -693,7 +698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="25.5">
+    <row r="7" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -705,7 +710,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="8" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -719,7 +724,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -733,7 +738,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -747,7 +752,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
@@ -761,7 +766,7 @@
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
@@ -775,7 +780,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
@@ -785,13 +790,13 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="25.5">
+    <row r="15" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
@@ -801,7 +806,7 @@
       </c>
       <c r="D15" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row r="16" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
@@ -815,7 +820,7 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>45</v>
       </c>
@@ -829,7 +834,7 @@
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>49</v>
       </c>
@@ -843,7 +848,7 @@
         <v>52</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>53</v>
       </c>
@@ -857,7 +862,7 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>56</v>
       </c>
@@ -871,7 +876,7 @@
         <v>59</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>60</v>
       </c>
@@ -881,7 +886,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>62</v>
       </c>
@@ -891,7 +896,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="25.5">
+    <row r="23" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>64</v>
       </c>
@@ -901,7 +906,7 @@
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row r="24" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>66</v>
       </c>
@@ -911,7 +916,7 @@
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
@@ -919,7 +924,7 @@
       </c>
       <c r="D25" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
@@ -927,7 +932,7 @@
       </c>
       <c r="D26" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
@@ -935,7 +940,7 @@
       </c>
       <c r="D27" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
@@ -943,7 +948,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
@@ -951,7 +956,7 @@
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
@@ -959,13 +964,14 @@
       </c>
       <c r="D30" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="95" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed killall to pkill on Cheat_Sheet
</commit_message>
<xml_diff>
--- a/documentation/Cheat_Sheet.xlsx
+++ b/documentation/Cheat_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevSRClocal\UX\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE77878-0F47-4363-8D59-38870BD2CC96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF65247-46CD-40EA-AA6D-6179A3DFE5B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9720" yWindow="4830" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,9 +109,6 @@
     <t>get the full path of program</t>
   </si>
   <si>
-    <t>killall</t>
-  </si>
-  <si>
     <t>kill by name</t>
   </si>
   <si>
@@ -245,6 +242,9 @@
   </si>
   <si>
     <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>pkill name</t>
   </si>
 </sst>
 </file>
@@ -677,7 +677,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
@@ -694,7 +694,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>8</v>
@@ -708,10 +708,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>11</v>
@@ -797,10 +797,10 @@
         <v>26</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -808,16 +808,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="C11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -825,11 +825,11 @@
     </row>
     <row r="12" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="5"/>
@@ -838,16 +838,16 @@
     </row>
     <row r="13" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -855,16 +855,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -872,16 +872,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -889,16 +889,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -906,16 +906,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -923,13 +923,13 @@
     </row>
     <row r="18" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="5"/>
@@ -938,16 +938,16 @@
     </row>
     <row r="19" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="C19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -955,16 +955,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -972,10 +972,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1048,10 +1048,10 @@
     </row>
     <row r="29" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>

</xml_diff>

<commit_message>
added Mignight commander to all releases
</commit_message>
<xml_diff>
--- a/documentation/Cheat_Sheet.xlsx
+++ b/documentation/Cheat_Sheet.xlsx
@@ -5,22 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevSRClocal\UX\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevSrcLocal\UX\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF65247-46CD-40EA-AA6D-6179A3DFE5B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B90C91-26AD-4645-AC6E-B53D4A7A52FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9720" yWindow="4830" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
   <si>
     <t>System-UX</t>
   </si>
@@ -245,6 +245,24 @@
   </si>
   <si>
     <t>pkill name</t>
+  </si>
+  <si>
+    <t>fte</t>
+  </si>
+  <si>
+    <t>IDE/Text Editor</t>
+  </si>
+  <si>
+    <t>mc</t>
+  </si>
+  <si>
+    <t>mcedit</t>
+  </si>
+  <si>
+    <t>Text Editor</t>
+  </si>
+  <si>
+    <t>File Explorer (Norton Commander Like)</t>
   </si>
 </sst>
 </file>
@@ -636,17 +654,19 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -659,7 +679,7 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -672,7 +692,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -689,7 +709,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -706,7 +726,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>70</v>
       </c>
@@ -723,7 +743,7 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -738,7 +758,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -755,7 +775,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -772,7 +792,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -789,7 +809,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
@@ -806,7 +826,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>74</v>
       </c>
@@ -823,7 +843,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -836,7 +856,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>35</v>
       </c>
@@ -853,7 +873,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>39</v>
       </c>
@@ -870,7 +890,7 @@
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -887,7 +907,7 @@
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>47</v>
       </c>
@@ -904,7 +924,7 @@
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>50</v>
       </c>
@@ -921,7 +941,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>54</v>
       </c>
@@ -936,7 +956,7 @@
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>56</v>
       </c>
@@ -953,7 +973,7 @@
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>58</v>
       </c>
@@ -970,47 +990,57 @@
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1019,7 +1049,7 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1028,7 +1058,7 @@
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1037,7 +1067,7 @@
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1046,7 +1076,7 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>59</v>
       </c>
@@ -1059,7 +1089,7 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>